<commit_message>
Make file read-only again
</commit_message>
<xml_diff>
--- a/Armins denk-o-mat - mobile Version.xlsx
+++ b/Armins denk-o-mat - mobile Version.xlsx
@@ -298,21 +298,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -892,10 +892,10 @@
       <c r="AV2" s="3"/>
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
-      <c r="BA2" s="11">
+      <c r="BA2" s="10">
         <v>1</v>
       </c>
-      <c r="BB2" s="10" t="s">
+      <c r="BB2" s="12" t="s">
         <v>49</v>
       </c>
     </row>
@@ -950,8 +950,8 @@
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
-      <c r="BA3" s="11"/>
-      <c r="BB3" s="10"/>
+      <c r="BA3" s="10"/>
+      <c r="BB3" s="12"/>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1004,8 +1004,8 @@
       <c r="AV4" s="3"/>
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
-      <c r="BA4" s="11"/>
-      <c r="BB4" s="10"/>
+      <c r="BA4" s="10"/>
+      <c r="BB4" s="12"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -1058,8 +1058,8 @@
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
-      <c r="BA5" s="11"/>
-      <c r="BB5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="12"/>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1112,8 +1112,8 @@
       <c r="AV6" s="3"/>
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
-      <c r="BA6" s="11"/>
-      <c r="BB6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="12"/>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1166,8 +1166,8 @@
       <c r="AV7" s="3"/>
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
-      <c r="BA7" s="11"/>
-      <c r="BB7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="12"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1220,8 +1220,8 @@
       <c r="AV8" s="3"/>
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
-      <c r="BA8" s="11"/>
-      <c r="BB8" s="10"/>
+      <c r="BA8" s="10"/>
+      <c r="BB8" s="12"/>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1274,8 +1274,8 @@
       <c r="AV9" s="3"/>
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
-      <c r="BA9" s="11"/>
-      <c r="BB9" s="10"/>
+      <c r="BA9" s="10"/>
+      <c r="BB9" s="12"/>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1328,8 +1328,8 @@
       <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
-      <c r="BA10" s="11"/>
-      <c r="BB10" s="10"/>
+      <c r="BA10" s="10"/>
+      <c r="BB10" s="12"/>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -1382,8 +1382,8 @@
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
-      <c r="BA11" s="11"/>
-      <c r="BB11" s="10"/>
+      <c r="BA11" s="10"/>
+      <c r="BB11" s="12"/>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1402,7 +1402,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1419,7 +1419,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
@@ -1433,7 +1433,7 @@
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL12" s="3"/>
       <c r="AM12" s="3"/>
@@ -1446,13 +1446,13 @@
       <c r="AT12" s="3"/>
       <c r="AU12" s="3">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV12" s="3"/>
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
-      <c r="BA12" s="11"/>
-      <c r="BB12" s="10"/>
+      <c r="BA12" s="10"/>
+      <c r="BB12" s="12"/>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -1471,7 +1471,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3" t="str">
         <f ca="1">INDEX(O15:O20,O12)</f>
-        <v>sechs-</v>
+        <v>zwei-</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1488,7 +1488,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3" t="str">
         <f ca="1">INDEX(Z15:Z20,Z12)</f>
-        <v>unumkehrbare/n</v>
+        <v>intransparente/n</v>
       </c>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
@@ -1502,7 +1502,7 @@
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3" t="str">
         <f ca="1">INDEX(AK15:AK20,AK12)</f>
-        <v>Wende-</v>
+        <v>Ehren-</v>
       </c>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
@@ -1515,13 +1515,13 @@
       <c r="AT13" s="3"/>
       <c r="AU13" s="3" t="str">
         <f ca="1">INDEX(AU15:AU20,AU12)</f>
-        <v>Sprint</v>
+        <v>Kampange</v>
       </c>
       <c r="AV13" s="3"/>
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
-      <c r="BA13" s="11"/>
-      <c r="BB13" s="10"/>
+      <c r="BA13" s="10"/>
+      <c r="BB13" s="12"/>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1574,8 +1574,8 @@
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
       <c r="AX14" s="3"/>
-      <c r="BA14" s="11"/>
-      <c r="BB14" s="10"/>
+      <c r="BA14" s="10"/>
+      <c r="BB14" s="12"/>
     </row>
     <row r="15" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -1638,8 +1638,8 @@
       <c r="AV15" s="9"/>
       <c r="AW15" s="9"/>
       <c r="AX15" s="3"/>
-      <c r="BA15" s="11"/>
-      <c r="BB15" s="10"/>
+      <c r="BA15" s="10"/>
+      <c r="BB15" s="12"/>
     </row>
     <row r="16" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -1702,8 +1702,8 @@
       <c r="AV16" s="9"/>
       <c r="AW16" s="9"/>
       <c r="AX16" s="3"/>
-      <c r="BA16" s="11"/>
-      <c r="BB16" s="10"/>
+      <c r="BA16" s="10"/>
+      <c r="BB16" s="12"/>
     </row>
     <row r="17" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1766,8 +1766,8 @@
       <c r="AV17" s="9"/>
       <c r="AW17" s="9"/>
       <c r="AX17" s="3"/>
-      <c r="BA17" s="11"/>
-      <c r="BB17" s="10"/>
+      <c r="BA17" s="10"/>
+      <c r="BB17" s="12"/>
     </row>
     <row r="18" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1830,8 +1830,8 @@
       <c r="AV18" s="9"/>
       <c r="AW18" s="9"/>
       <c r="AX18" s="3"/>
-      <c r="BA18" s="11"/>
-      <c r="BB18" s="10"/>
+      <c r="BA18" s="10"/>
+      <c r="BB18" s="12"/>
     </row>
     <row r="19" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1894,8 +1894,8 @@
       <c r="AV19" s="9"/>
       <c r="AW19" s="9"/>
       <c r="AX19" s="3"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="10"/>
+      <c r="BA19" s="10"/>
+      <c r="BB19" s="12"/>
     </row>
     <row r="20" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1958,8 +1958,8 @@
       <c r="AV20" s="9"/>
       <c r="AW20" s="9"/>
       <c r="AX20" s="3"/>
-      <c r="BA20" s="11"/>
-      <c r="BB20" s="10"/>
+      <c r="BA20" s="10"/>
+      <c r="BB20" s="12"/>
     </row>
     <row r="21" spans="1:54" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -2012,8 +2012,8 @@
       <c r="AV21" s="3"/>
       <c r="AW21" s="3"/>
       <c r="AX21" s="3"/>
-      <c r="BA21" s="11"/>
-      <c r="BB21" s="10"/>
+      <c r="BA21" s="10"/>
+      <c r="BB21" s="12"/>
     </row>
     <row r="22" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -2076,8 +2076,8 @@
       <c r="AX22" s="4"/>
       <c r="AY22" s="2"/>
       <c r="AZ22" s="2"/>
-      <c r="BA22" s="11"/>
-      <c r="BB22" s="10"/>
+      <c r="BA22" s="10"/>
+      <c r="BB22" s="12"/>
     </row>
     <row r="23" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -2140,8 +2140,8 @@
       <c r="AX23" s="4"/>
       <c r="AY23" s="2"/>
       <c r="AZ23" s="2"/>
-      <c r="BA23" s="11"/>
-      <c r="BB23" s="10"/>
+      <c r="BA23" s="10"/>
+      <c r="BB23" s="12"/>
     </row>
     <row r="24" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -2204,8 +2204,8 @@
       <c r="AX24" s="4"/>
       <c r="AY24" s="2"/>
       <c r="AZ24" s="2"/>
-      <c r="BA24" s="11"/>
-      <c r="BB24" s="10"/>
+      <c r="BA24" s="10"/>
+      <c r="BB24" s="12"/>
     </row>
     <row r="25" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2268,8 +2268,8 @@
       <c r="AX25" s="4"/>
       <c r="AY25" s="2"/>
       <c r="AZ25" s="2"/>
-      <c r="BA25" s="11"/>
-      <c r="BB25" s="10"/>
+      <c r="BA25" s="10"/>
+      <c r="BB25" s="12"/>
     </row>
     <row r="26" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -2332,8 +2332,8 @@
       <c r="AX26" s="4"/>
       <c r="AY26" s="2"/>
       <c r="AZ26" s="2"/>
-      <c r="BA26" s="11"/>
-      <c r="BB26" s="10"/>
+      <c r="BA26" s="10"/>
+      <c r="BB26" s="12"/>
     </row>
     <row r="27" spans="1:54" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -2396,8 +2396,8 @@
       <c r="AX27" s="4"/>
       <c r="AY27" s="2"/>
       <c r="AZ27" s="2"/>
-      <c r="BA27" s="11"/>
-      <c r="BB27" s="10"/>
+      <c r="BA27" s="10"/>
+      <c r="BB27" s="12"/>
     </row>
     <row r="28" spans="1:54" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -2450,101 +2450,101 @@
       <c r="AV28" s="3"/>
       <c r="AW28" s="3"/>
       <c r="AX28" s="3"/>
-      <c r="BA28" s="11"/>
-      <c r="BB28" s="10"/>
+      <c r="BA28" s="10"/>
+      <c r="BB28" s="12"/>
     </row>
     <row r="29" spans="1:54" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S29" s="1">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AD29" s="1">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AR29" s="1">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="1">
+      <c r="E30" s="1" t="str">
         <f ca="1">INDEX(E22:E27,E29)</f>
-        <v>2030</v>
+        <v>auf Weiteres</v>
       </c>
       <c r="S30" s="1" t="str">
         <f ca="1">INDEX(S22:S27,S29)</f>
-        <v>willkürlichen</v>
+        <v>allmählichen</v>
       </c>
       <c r="AD30" s="1" t="str">
         <f ca="1">INDEX(AD22:AD27,AD29)</f>
-        <v>Beschönigung</v>
+        <v>Senkung</v>
       </c>
       <c r="AR30" s="1" t="str">
         <f ca="1">INDEX(AR22:AR27,AR29)</f>
-        <v>Beschönigung</v>
+        <v>Steigerung</v>
       </c>
     </row>
     <row r="32" spans="1:54" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="11" t="str">
         <f ca="1">"Was wir jetzt brauchen, ist ein/e " &amp; O13 &amp; " " &amp; T13 &amp; " " &amp; Z13 &amp; " "  &amp; AK13 &amp; " " &amp; AU13  &amp; " bis " &amp;E30 &amp; " zur " &amp; S30&amp; " "  &amp; AD30 &amp; " der " &amp;AR30</f>
-        <v>Was wir jetzt brauchen, ist ein/e sechs- fache/n unumkehrbare/n Wende- Sprint bis 2030 zur willkürlichen Beschönigung der Beschönigung</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
-      <c r="AD32" s="8"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="8"/>
-      <c r="AI32" s="8"/>
-      <c r="AJ32" s="8"/>
-      <c r="AK32" s="8"/>
-      <c r="AL32" s="8"/>
-      <c r="AM32" s="8"/>
-      <c r="AN32" s="8"/>
-      <c r="AO32" s="8"/>
-      <c r="AP32" s="8"/>
-      <c r="AQ32" s="8"/>
-      <c r="AR32" s="8"/>
-      <c r="AS32" s="8"/>
-      <c r="AT32" s="8"/>
-      <c r="AU32" s="8"/>
-      <c r="AV32" s="8"/>
-      <c r="AW32" s="8"/>
-      <c r="AX32" s="8"/>
-      <c r="AY32" s="8"/>
-      <c r="AZ32" s="12"/>
+        <v>Was wir jetzt brauchen, ist ein/e zwei- fache/n intransparente/n Ehren- Kampange bis auf Weiteres zur allmählichen Senkung der Steigerung</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="11"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="11"/>
+      <c r="AJ32" s="11"/>
+      <c r="AK32" s="11"/>
+      <c r="AL32" s="11"/>
+      <c r="AM32" s="11"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="11"/>
+      <c r="AP32" s="11"/>
+      <c r="AQ32" s="11"/>
+      <c r="AR32" s="11"/>
+      <c r="AS32" s="11"/>
+      <c r="AT32" s="11"/>
+      <c r="AU32" s="11"/>
+      <c r="AV32" s="11"/>
+      <c r="AW32" s="11"/>
+      <c r="AX32" s="11"/>
+      <c r="AY32" s="11"/>
+      <c r="AZ32" s="8"/>
     </row>
     <row r="34" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
@@ -2579,12 +2579,33 @@
       <c r="AA34" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="57">
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="BA2:BA28"/>
+    <mergeCell ref="A32:AY32"/>
+    <mergeCell ref="BB2:BB28"/>
+    <mergeCell ref="AR26:AV26"/>
+    <mergeCell ref="AR27:AV27"/>
+    <mergeCell ref="AU15:AW15"/>
+    <mergeCell ref="AU16:AW16"/>
+    <mergeCell ref="AU17:AW17"/>
+    <mergeCell ref="AU18:AW18"/>
+    <mergeCell ref="AU19:AW19"/>
+    <mergeCell ref="AU20:AW20"/>
+    <mergeCell ref="AR22:AV22"/>
+    <mergeCell ref="AR23:AV23"/>
+    <mergeCell ref="AR24:AV24"/>
+    <mergeCell ref="AR25:AV25"/>
+    <mergeCell ref="AK15:AQ15"/>
+    <mergeCell ref="AK16:AQ16"/>
+    <mergeCell ref="AD24:AK24"/>
+    <mergeCell ref="AD25:AK25"/>
+    <mergeCell ref="AD26:AK26"/>
+    <mergeCell ref="AD27:AK27"/>
+    <mergeCell ref="AK17:AQ17"/>
+    <mergeCell ref="AK18:AQ18"/>
+    <mergeCell ref="AK19:AQ19"/>
+    <mergeCell ref="AK20:AQ20"/>
+    <mergeCell ref="AD22:AK22"/>
     <mergeCell ref="E26:L26"/>
     <mergeCell ref="E27:L27"/>
     <mergeCell ref="T15:W15"/>
@@ -2601,6 +2622,11 @@
     <mergeCell ref="E25:L25"/>
     <mergeCell ref="O15:Q15"/>
     <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="BA2:BA28"/>
     <mergeCell ref="S24:Z24"/>
     <mergeCell ref="S25:Z25"/>
     <mergeCell ref="S26:Z26"/>
@@ -2612,31 +2638,6 @@
     <mergeCell ref="Z19:AF19"/>
     <mergeCell ref="Z20:AF20"/>
     <mergeCell ref="AD23:AK23"/>
-    <mergeCell ref="AD24:AK24"/>
-    <mergeCell ref="AD25:AK25"/>
-    <mergeCell ref="AD26:AK26"/>
-    <mergeCell ref="AD27:AK27"/>
-    <mergeCell ref="AK17:AQ17"/>
-    <mergeCell ref="AK18:AQ18"/>
-    <mergeCell ref="AK19:AQ19"/>
-    <mergeCell ref="AK20:AQ20"/>
-    <mergeCell ref="AD22:AK22"/>
-    <mergeCell ref="A32:AY32"/>
-    <mergeCell ref="BB2:BB28"/>
-    <mergeCell ref="AR26:AV26"/>
-    <mergeCell ref="AR27:AV27"/>
-    <mergeCell ref="AU15:AW15"/>
-    <mergeCell ref="AU16:AW16"/>
-    <mergeCell ref="AU17:AW17"/>
-    <mergeCell ref="AU18:AW18"/>
-    <mergeCell ref="AU19:AW19"/>
-    <mergeCell ref="AU20:AW20"/>
-    <mergeCell ref="AR22:AV22"/>
-    <mergeCell ref="AR23:AV23"/>
-    <mergeCell ref="AR24:AV24"/>
-    <mergeCell ref="AR25:AV25"/>
-    <mergeCell ref="AK15:AQ15"/>
-    <mergeCell ref="AK16:AQ16"/>
   </mergeCells>
   <conditionalFormatting sqref="O15:O20 T15:T20 Z15:Z20 AK15:AK20 AU15:AU20">
     <cfRule type="expression" dxfId="4" priority="5">

</xml_diff>